<commit_message>
addind preparer to sheet
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_0629_0618.xlsx
+++ b/fastqFiles/fastq_0629_0618.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/fastqFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B0DBA4D-B41C-E640-AA84-5D20D4C0578E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293ADB27-509F-5E44-A860-AC5D8294CF4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="21060" windowHeight="13340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="35">
   <si>
     <t>libraryDate</t>
   </si>
@@ -122,6 +122,9 @@
   </si>
   <si>
     <t>S.GISH</t>
+  </si>
+  <si>
+    <t>fullRNASEQ</t>
   </si>
 </sst>
 </file>
@@ -488,7 +491,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" activeCellId="1" sqref="B3:B25 E2:E25"/>
+      <selection activeCell="E24" sqref="E24:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -527,7 +530,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -547,7 +550,7 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
@@ -567,7 +570,7 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -587,7 +590,7 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
@@ -607,7 +610,7 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
         <v>13</v>
@@ -627,7 +630,7 @@
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -647,7 +650,7 @@
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F8" t="s">
         <v>15</v>
@@ -667,7 +670,7 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F9" t="s">
         <v>16</v>
@@ -687,7 +690,7 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F10" t="s">
         <v>17</v>
@@ -707,7 +710,7 @@
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
         <v>18</v>
@@ -727,7 +730,7 @@
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F12" t="s">
         <v>19</v>
@@ -747,7 +750,7 @@
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
@@ -767,7 +770,7 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F14" t="s">
         <v>21</v>
@@ -787,7 +790,7 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F15" t="s">
         <v>22</v>
@@ -807,7 +810,7 @@
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F16" t="s">
         <v>23</v>
@@ -827,7 +830,7 @@
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F17" t="s">
         <v>24</v>
@@ -847,7 +850,7 @@
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F18" t="s">
         <v>25</v>
@@ -867,7 +870,7 @@
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
         <v>26</v>
@@ -887,7 +890,7 @@
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F20" t="s">
         <v>27</v>
@@ -907,7 +910,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F21" t="s">
         <v>28</v>
@@ -927,7 +930,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
         <v>29</v>
@@ -947,7 +950,7 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F23" t="s">
         <v>30</v>
@@ -967,7 +970,7 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F24" t="s">
         <v>31</v>
@@ -987,7 +990,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F25" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
remove containing path to fastq filenames
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_0629_0618.xlsx
+++ b/fastqFiles/fastq_0629_0618.xlsx
@@ -52,79 +52,79 @@
     <t xml:space="preserve">fullRNASEQ</t>
   </si>
   <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_AAATGCA.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_ACAGATA.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_ACGCGGG.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_ACTGTCG.fastq.gz</t>
+    <t xml:space="preserve">run_0629_0618_sequence_AAATGCA.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_ACAGATA.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_ACGCGGG.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_ACTGTCG.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">10.19.11</t>
   </si>
   <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_AGACTGA.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_ATCGAGC.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_ATGACAG.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_CACCTCC.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_CCATCAT.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_CCGATTA.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_CGGTGGC.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_CTCAATG.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_CTTGGAA.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_GAGGCGT.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_GAGTACG.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_GCTTAGA.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_GGAGTCC.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_GGCAGCG.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_GGTCCTC.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_GTATTTG.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_TAACAAG.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_TACTCTA.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_TGAGGTT.fastq.gz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sequence/run_0629_0618_pooled/run_0629_0618_sequence_TTTAACT.fastq.gz</t>
+    <t xml:space="preserve">run_0629_0618_sequence_AGACTGA.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_ATCGAGC.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_ATGACAG.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_CACCTCC.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_CCATCAT.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_CCGATTA.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_CGGTGGC.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_CTCAATG.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_CTTGGAA.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_GAGGCGT.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_GAGTACG.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_GCTTAGA.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_GGAGTCC.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_GGCAGCG.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_GGTCCTC.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_GTATTTG.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_TAACAAG.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_TACTCTA.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_TGAGGTT.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">run_0629_0618_sequence_TTTAACT.fastq.gz</t>
   </si>
 </sst>
 </file>
@@ -243,7 +243,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
fixing formating on fastq purpose column
</commit_message>
<xml_diff>
--- a/fastqFiles/fastq_0629_0618.xlsx
+++ b/fastqFiles/fastq_0629_0618.xlsx
@@ -444,7 +444,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -479,7 +479,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -514,7 +514,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -549,7 +549,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -584,7 +584,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -619,7 +619,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -654,7 +654,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -689,7 +689,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -724,7 +724,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -794,7 +794,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -829,7 +829,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -864,7 +864,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -899,7 +899,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -934,7 +934,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -969,7 +969,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1004,7 +1004,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -1074,7 +1074,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -1109,7 +1109,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -1144,7 +1144,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -1179,7 +1179,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1214,7 +1214,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -1249,7 +1249,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>fullRNASEQ</t>
+          <t>fullRNASeq</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">

</xml_diff>